<commit_message>
Update 24 Feb 2023
</commit_message>
<xml_diff>
--- a/BirthdayFile.xlsx
+++ b/BirthdayFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yokvachuk\Desktop\Files\Enternainwork\Arbeit\41. Birthday_reminder\Birthday_reminder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633270E8-B398-46CB-9EE2-E634D63B67CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657C96D3-F532-4BFD-AD8C-CC1A0D975DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="192" yWindow="204" windowWidth="9600" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birthdays" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Joseph Biden</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Geral Ford</t>
+  </si>
+  <si>
+    <t>George Bush</t>
+  </si>
+  <si>
+    <t>Bill Clinton</t>
   </si>
 </sst>
 </file>
@@ -385,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,6 +515,22 @@
         <v>4185</v>
       </c>
     </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>32197</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>28545</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update (5 April 2023)
</commit_message>
<xml_diff>
--- a/BirthdayFile.xlsx
+++ b/BirthdayFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yokvachuk\Desktop\Files\Enternainwork\Arbeit\41. Birthday_reminder\Birthday_reminder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive-global.kpmg.com/personal/yokvachuk_kpmg_ua/Documents/Desktop/Files/Enternainwork/Arbeit/41. Birthday_reminder/Birthday_reminder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{657C96D3-F532-4BFD-AD8C-CC1A0D975DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{657C96D3-F532-4BFD-AD8C-CC1A0D975DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE1DB0A5-75C9-469A-87D4-2568CC0453AD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32400" yWindow="2820" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birthdays" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Joseph Biden</t>
   </si>
@@ -73,6 +73,27 @@
   </si>
   <si>
     <t>Bill Clinton</t>
+  </si>
+  <si>
+    <t>Andrew Jackson</t>
+  </si>
+  <si>
+    <t>Jimmy Carther</t>
+  </si>
+  <si>
+    <t>Ronald Reigan</t>
+  </si>
+  <si>
+    <t>Lyndon Johnson</t>
+  </si>
+  <si>
+    <t>Woodrow Wilson</t>
+  </si>
+  <si>
+    <t>Warren Harding</t>
+  </si>
+  <si>
+    <t>Calvin Coolidge</t>
   </si>
 </sst>
 </file>
@@ -391,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -531,6 +552,62 @@
         <v>28545</v>
       </c>
     </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>7765</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="1">
+        <v>29680</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="1">
+        <v>31505</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="1">
+        <v>33334</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>33335</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>36625</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1">
+        <v>31875</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update 14 April 2023 (works)
</commit_message>
<xml_diff>
--- a/BirthdayFile.xlsx
+++ b/BirthdayFile.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive-global.kpmg.com/personal/yokvachuk_kpmg_ua/Documents/Desktop/Files/Enternainwork/Arbeit/41. Birthday_reminder/Birthday_reminder/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yokvachuk\Desktop\Files\Enternainwork\Arbeit\41. Birthday_reminder\Birthday_reminder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{657C96D3-F532-4BFD-AD8C-CC1A0D975DDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE1DB0A5-75C9-469A-87D4-2568CC0453AD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B4DE25-69EC-482E-AC5A-519729CD8C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32400" yWindow="2820" windowWidth="17280" windowHeight="8976" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Birthdays" sheetId="1" r:id="rId1"/>
+    <sheet name="Birthdays (2)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
   <si>
     <t>Joseph Biden</t>
   </si>
@@ -94,16 +95,105 @@
   </si>
   <si>
     <t>Calvin Coolidge</t>
+  </si>
+  <si>
+    <t>Jbiden@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Jadams@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Jbuchanan@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Jcarther@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Bobama@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Gwashington@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Dtrump@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Hhoover@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Tjeffeston@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Mburen@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Wharrison@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Fpierce@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Alincoln@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Ajohnson@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Gford@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Gbush@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Bclinton@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Ajackson@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Ljohnson@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Rreigan@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Wwilson@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Wharding@whitehouse.com</t>
+  </si>
+  <si>
+    <t>Ccoolidge@whitehouse.com</t>
+  </si>
+  <si>
+    <t>User 1</t>
+  </si>
+  <si>
+    <t>User 2</t>
+  </si>
+  <si>
+    <t>yokvachuk@kpmg.com</t>
+  </si>
+  <si>
+    <t>avoinalovych@kpmg.ua</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,14 +216,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -412,203 +505,452 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1">
+        <v>7775</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1">
+        <v>29690</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>31515</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1">
+        <v>33344</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>33342</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1">
+        <v>36626</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1">
+        <v>31878</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="1">
+        <v>37057</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="1">
+        <v>32948</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{15309732-6961-49C5-9B09-1ED6ACEDA6E6}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{9AFF2F29-5074-46A3-962C-7B79F3588462}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{904400D6-6A71-494E-BAAD-F1C9C6D87B21}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{87F9059E-C13A-446F-88D8-AB6B581EFB81}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{E4E26FEA-C1E7-4509-BB1D-6CCD9ACCD9DF}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{7004B8B3-5115-4E2C-BE5C-0EF03FCE8222}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{E0B3ED5C-FCB2-42C2-A66A-A4C5A11C9D40}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{2572137E-792A-430B-816E-F5285C43F35E}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{5044DCBC-F4AD-4ED3-A409-BD9040778BD7}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E4CE518-E5B4-4924-AA83-26F7F81693B7}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
         <v>15665</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>22497</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>4071</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>16967</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>27251</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>44978</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>44979</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>31836</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>23800</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>20151</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C10" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>20437</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>29738</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>29606</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C13" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>4185</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C14" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>32197</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C15" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>28545</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C16" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1">
-        <v>7765</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+        <v>7775</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1">
-        <v>29680</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+        <v>29690</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19" s="1">
-        <v>31505</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+        <v>31515</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="1">
-        <v>33334</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33344</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>33335</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+        <v>33342</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1">
-        <v>36625</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+        <v>36626</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="1">
-        <v>31875</v>
+        <v>31878</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1">
+        <v>37057</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1">
+        <v>32948</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" xr:uid="{BFF29D2D-FC7B-425F-8A90-EF70EC9B413B}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{5C5BCB0F-FC8B-4303-B09D-4AF62CC7D13E}"/>
+    <hyperlink ref="C3" r:id="rId3" xr:uid="{14F6002F-7CFA-414E-8C76-2C10350B4418}"/>
+    <hyperlink ref="C4" r:id="rId4" xr:uid="{22F08C52-9349-48FC-A799-E46AE4AB8165}"/>
+    <hyperlink ref="C5" r:id="rId5" xr:uid="{D92A0CA7-E721-495E-AD09-579B8EF6FB83}"/>
+    <hyperlink ref="C6" r:id="rId6" xr:uid="{465A74B2-8E7A-4B69-989B-4513244F73D1}"/>
+    <hyperlink ref="C7" r:id="rId7" xr:uid="{B005F98C-2FA0-4B39-9D8F-D19A84493969}"/>
+    <hyperlink ref="C8" r:id="rId8" xr:uid="{C7B0B070-6D9E-4A3D-8BE6-03739AB55638}"/>
+    <hyperlink ref="C9" r:id="rId9" xr:uid="{5CB675B2-5AFE-4EBD-A45A-971F1FB60715}"/>
+    <hyperlink ref="C10" r:id="rId10" xr:uid="{0D8962FD-0225-4904-98C2-5DBF26CE28AB}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{85E9913A-CFA2-4316-A070-B52C3861F186}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{C0E81317-0553-4A7A-8595-05DD07675E4E}"/>
+    <hyperlink ref="C13" r:id="rId13" xr:uid="{D828DCAE-B032-4AA9-9778-F927C88B2F7B}"/>
+    <hyperlink ref="C14" r:id="rId14" xr:uid="{85BA12A4-2D12-49F2-9DA4-42FC4F490682}"/>
+    <hyperlink ref="C15" r:id="rId15" xr:uid="{6CBB4E33-B461-47AD-B5B0-078FEAA3BE35}"/>
+    <hyperlink ref="C16" r:id="rId16" xr:uid="{D444E5F3-53DF-4D2E-9D12-26804498888C}"/>
+    <hyperlink ref="C17" r:id="rId17" xr:uid="{F934DFE1-1025-4830-B84F-F36CBCF2C8F2}"/>
+    <hyperlink ref="C18" r:id="rId18" xr:uid="{1C17CCC0-E665-4123-81F8-C6A0EF2776CB}"/>
+    <hyperlink ref="C19" r:id="rId19" xr:uid="{D82C2345-4773-482B-A8AE-1CCC54322E28}"/>
+    <hyperlink ref="C20" r:id="rId20" xr:uid="{C9B8C9C4-5D49-42A8-97FA-BBAED73B190A}"/>
+    <hyperlink ref="C21" r:id="rId21" xr:uid="{7AAB93D1-2FD8-4AD5-BC66-47E56376B3AB}"/>
+    <hyperlink ref="C22" r:id="rId22" xr:uid="{F6DC5A25-EDE9-4FA4-BDF0-6449B1BC91CC}"/>
+    <hyperlink ref="C23" r:id="rId23" xr:uid="{5A3F596D-800B-4A7D-A80E-34B82E1CF890}"/>
+    <hyperlink ref="C25" r:id="rId24" xr:uid="{69F88CAE-C30F-4EB1-8F6B-049B3F597FF4}"/>
+    <hyperlink ref="C24" r:id="rId25" xr:uid="{89D0AC4D-89B0-42EB-8319-3DDE19157BFC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>